<commit_message>
Update to FTT-H standalone
Updating FTT-H to align with Fortran updates. Mostly updates to csv files,  but also update to variable names in standalone code and some additional steps in variable calculation
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E3ME\FTT_Stand_Alone\Inputs\_MasterFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ae476_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEBDAB1B-EDBE-4931-B363-6A3441B853F4}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -965,10 +965,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -986,6 +985,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1257,16 +1260,16 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.59765625" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.86328125" customWidth="1"/>
-    <col min="7" max="7" width="14.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1292,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -1473,7 +1476,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1496,7 +1499,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -1519,7 +1522,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -1634,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1680,7 +1683,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1722,14 +1725,14 @@
       <selection activeCell="A2" sqref="A2:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.59765625" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1752,7 +1755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1821,7 +1824,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1844,7 +1847,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1890,7 +1893,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1936,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1959,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2051,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2074,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2120,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2143,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2189,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2212,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -2235,7 +2238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2267,17 +2270,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893746F0-70F0-4C21-8E46-9B5DBA6E54BB}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2300,7 +2303,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -2346,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -2369,7 +2372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -2392,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -2415,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -2484,7 +2487,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>109</v>
       </c>
@@ -2507,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -2530,7 +2533,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>111</v>
       </c>
@@ -2553,7 +2556,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -2576,7 +2579,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -2599,7 +2602,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -2622,7 +2625,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -2645,7 +2648,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -2681,14 +2684,14 @@
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.59765625" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2711,7 +2714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2734,7 +2737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -2757,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -2780,7 +2783,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2803,7 +2806,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>137</v>
       </c>
@@ -2826,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -2849,7 +2852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>139</v>
       </c>
@@ -2872,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>140</v>
       </c>
@@ -2895,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -2918,7 +2921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -2941,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -2964,7 +2967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>144</v>
       </c>
@@ -2987,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -3010,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -3033,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -3056,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>148</v>
       </c>
@@ -3079,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>149</v>
       </c>
@@ -3102,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>150</v>
       </c>
@@ -3125,7 +3128,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>151</v>
       </c>
@@ -3148,7 +3151,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>152</v>
       </c>
@@ -3171,7 +3174,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>153</v>
       </c>
@@ -3194,7 +3197,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>154</v>
       </c>
@@ -3217,7 +3220,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>155</v>
       </c>
@@ -3240,7 +3243,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>156</v>
       </c>
@@ -3272,21 +3275,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.06640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3315,7 +3318,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>189</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3373,7 +3376,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -3395,14 +3398,14 @@
       <c r="G4" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>220</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>198</v>
       </c>
@@ -3424,14 +3427,14 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>236</v>
       </c>
       <c r="I5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>201</v>
       </c>
@@ -3460,7 +3463,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>222</v>
       </c>
@@ -3489,7 +3492,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>224</v>
       </c>
@@ -3518,7 +3521,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>225</v>
       </c>
@@ -3547,7 +3550,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>226</v>
       </c>
@@ -3576,7 +3579,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>227</v>
       </c>
@@ -3605,7 +3608,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>228</v>
       </c>
@@ -3634,7 +3637,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>218</v>
       </c>
@@ -3663,7 +3666,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>232</v>
       </c>
@@ -3689,7 +3692,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>234</v>
       </c>
@@ -3715,7 +3718,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>241</v>
       </c>
@@ -3744,7 +3747,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>242</v>
       </c>
@@ -3773,14 +3776,14 @@
         <v>238</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>245</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>35340000</v>
       </c>
       <c r="D18" t="s">
@@ -3802,14 +3805,14 @@
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>251</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>35350000</v>
       </c>
       <c r="D19" t="s">
@@ -3831,7 +3834,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>253</v>
       </c>
@@ -3860,7 +3863,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>257</v>
       </c>
@@ -3889,14 +3892,14 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>261</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>35360000</v>
       </c>
       <c r="D22" t="s">
@@ -3905,7 +3908,7 @@
       <c r="E22" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>280</v>
       </c>
       <c r="G22">
@@ -3918,14 +3921,14 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>267</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>35370000</v>
       </c>
       <c r="D23" t="s">
@@ -3947,14 +3950,14 @@
         <v>266</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>273</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>35380000</v>
       </c>
       <c r="D24" t="s">
@@ -3976,7 +3979,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>269</v>
       </c>
@@ -3992,7 +3995,7 @@
       <c r="E25" t="s">
         <v>195</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" t="s">
         <v>41</v>
       </c>
       <c r="G25">
@@ -4005,26 +4008,26 @@
         <v>275</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
         <v>279</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>35390000</v>
       </c>
       <c r="D26" t="s">
         <v>276</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>56</v>
       </c>
       <c r="H26" t="s">
@@ -4034,17 +4037,17 @@
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>284</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>35410000</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>287</v>
       </c>
       <c r="E27" t="s">
@@ -4072,13 +4075,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4086,7 +4089,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4094,7 +4097,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4102,7 +4105,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4110,7 +4113,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4118,7 +4121,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4126,7 +4129,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -4134,7 +4137,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4142,7 +4145,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4150,7 +4153,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4158,7 +4161,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4166,7 +4169,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -4174,7 +4177,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -4182,7 +4185,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -4190,7 +4193,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -4198,7 +4201,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -4206,7 +4209,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -4214,7 +4217,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -4222,7 +4225,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -4230,7 +4233,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -4238,7 +4241,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -4246,7 +4249,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -4254,7 +4257,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -4262,7 +4265,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -4270,7 +4273,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>107</v>
       </c>
@@ -4278,7 +4281,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>108</v>
       </c>
@@ -4286,7 +4289,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -4294,7 +4297,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -4302,7 +4305,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -4310,7 +4313,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -4318,7 +4321,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -4326,7 +4329,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -4334,7 +4337,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -4342,7 +4345,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -4350,7 +4353,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -4358,7 +4361,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -4366,7 +4369,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>135</v>
       </c>
@@ -4374,7 +4377,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4382,7 +4385,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4390,7 +4393,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4398,7 +4401,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4406,7 +4409,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4414,7 +4417,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>155</v>
       </c>
@@ -4422,7 +4425,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>156</v>
       </c>
@@ -4430,7 +4433,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>189</v>
       </c>
@@ -4438,7 +4441,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>192</v>
       </c>
@@ -4446,7 +4449,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>223</v>
       </c>
@@ -4454,7 +4457,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>198</v>
       </c>
@@ -4462,7 +4465,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>201</v>
       </c>
@@ -4470,7 +4473,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>222</v>
       </c>
@@ -4478,7 +4481,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>224</v>
       </c>
@@ -4486,7 +4489,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>225</v>
       </c>
@@ -4494,7 +4497,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>226</v>
       </c>
@@ -4502,7 +4505,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>227</v>
       </c>
@@ -4510,7 +4513,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>228</v>
       </c>
@@ -4518,7 +4521,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>218</v>
       </c>
@@ -4526,7 +4529,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>251</v>
       </c>
@@ -4534,7 +4537,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>253</v>
       </c>
@@ -4542,7 +4545,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>257</v>
       </c>
@@ -4550,7 +4553,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>273</v>
       </c>
@@ -4558,8 +4561,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" s="4"/>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Big update to new freight classification
Changing the technology classification of FTT-Freight to add vans and three-wheelers. Cost data and shares data is dummy.

This version successfully exports CSVs and the model runs. The shares equation is broken but learning and cumulative capacities appear to function as expected.

Some variables have been removed from the FTT-Freight Masterfile and  'VariableListing.csv' because they were not used. Some elements of the freight cost matrix have also been removed for the same reason.

Also some general formatting of the freight Masterfile.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{633FC2CE-8022-472C-9BE9-1C2649AABB15}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{752E57D9-DD86-4374-B143-621D1A74ADF5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="281">
   <si>
     <t>Variable name</t>
   </si>
@@ -689,9 +689,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>FTT-Fr Vehicle Sales</t>
-  </si>
-  <si>
     <t>ZREG</t>
   </si>
   <si>
@@ -722,9 +719,6 @@
     <t>REG</t>
   </si>
   <si>
-    <t>Xitot</t>
-  </si>
-  <si>
     <t>FTT-Fr Spillover Matrix</t>
   </si>
   <si>
@@ -749,18 +743,9 @@
     <t>FTT-Fr Exchange Matrix</t>
   </si>
   <si>
-    <t>Costs (Sales History)</t>
-  </si>
-  <si>
-    <t>XiH</t>
-  </si>
-  <si>
     <t>RVHH</t>
   </si>
   <si>
-    <t>FTT-Fr Sales History</t>
-  </si>
-  <si>
     <t>ZESF</t>
   </si>
   <si>
@@ -776,15 +761,6 @@
     <t>ZSFD</t>
   </si>
   <si>
-    <t>dEll</t>
-  </si>
-  <si>
-    <t>Costs (Survival Function Age Derivative)</t>
-  </si>
-  <si>
-    <t>FTT-Fr Survival Function Age Derivative</t>
-  </si>
-  <si>
     <t>ZLOD</t>
   </si>
   <si>
@@ -903,6 +879,12 @@
   </si>
   <si>
     <t>RZFT</t>
+  </si>
+  <si>
+    <t>ZEWW</t>
+  </si>
+  <si>
+    <t>FTT-Fr Cumulative Capacities</t>
   </si>
 </sst>
 </file>
@@ -1271,10 +1253,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1303,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1332,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1361,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1390,7 +1372,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1419,7 +1401,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1448,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1477,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1491,7 +1473,7 @@
         <v>31090000</v>
       </c>
       <c r="D9" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="E9" t="s">
         <v>56</v>
@@ -1506,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1535,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1564,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1593,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1622,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1651,7 +1633,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1680,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1709,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1738,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1767,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1796,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -1814,7 +1796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1848,10 +1830,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1877,10 +1859,10 @@
         <v>54</v>
       </c>
       <c r="H2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1909,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1938,7 +1920,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1967,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1996,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -2025,7 +2007,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -2054,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -2083,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2112,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -2141,7 +2123,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -2170,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -2199,7 +2181,7 @@
         <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -2228,7 +2210,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -2257,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -2286,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -2315,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -2344,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -2373,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -2402,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -2431,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -2460,7 +2442,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2505,10 +2487,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -2537,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2566,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -2595,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -2624,7 +2606,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -2653,7 +2635,7 @@
         <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -2682,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -2711,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -2740,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2769,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -2798,7 +2780,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -2827,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -2856,7 +2838,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -2885,7 +2867,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -2914,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -2943,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -2969,10 +2951,10 @@
         <v>54</v>
       </c>
       <c r="H17" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I17" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3018,10 +3000,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -3050,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3079,7 +3061,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -3108,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -3137,7 +3119,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -3166,7 +3148,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3195,7 +3177,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -3224,7 +3206,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -3253,7 +3235,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -3282,7 +3264,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3311,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -3340,7 +3322,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -3369,7 +3351,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -3398,7 +3380,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -3427,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -3456,7 +3438,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -3485,7 +3467,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -3514,7 +3496,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -3543,7 +3525,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -3572,7 +3554,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -3601,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -3630,7 +3612,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -3659,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -3688,7 +3670,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -3717,7 +3699,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3727,10 +3709,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3772,10 +3754,10 @@
         <v>188</v>
       </c>
       <c r="J1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="K1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -3810,7 +3792,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -3845,12 +3827,12 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3880,21 +3862,21 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>278</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>35070000</v>
+        <v>35140000</v>
       </c>
       <c r="D5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E5" t="s">
         <v>54</v>
@@ -3906,65 +3888,65 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="I5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>286</v>
+        <v>215</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>35140000</v>
+        <v>35040000</v>
       </c>
       <c r="D6" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="G6">
-        <v>0</v>
+      <c r="G6" t="s">
+        <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="I6" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>35040000</v>
+        <v>35050000</v>
       </c>
       <c r="D7" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="E7" t="s">
         <v>192</v>
@@ -3976,16 +3958,16 @@
         <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="I7" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -3996,10 +3978,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>35050000</v>
+        <v>35020000</v>
       </c>
       <c r="D8" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="E8" t="s">
         <v>192</v>
@@ -4011,16 +3993,16 @@
         <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="I8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -4031,10 +4013,10 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>35020000</v>
+        <v>35030000</v>
       </c>
       <c r="D9" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="E9" t="s">
         <v>192</v>
@@ -4046,16 +4028,16 @@
         <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="I9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -4066,31 +4048,31 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>35030000</v>
+        <v>35150000</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="E10" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="s">
-        <v>54</v>
+      <c r="G10">
+        <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="I10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -4101,10 +4083,10 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>35150000</v>
+        <v>35130000</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="E11" t="s">
         <v>54</v>
@@ -4116,65 +4098,65 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>210</v>
+        <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>35130000</v>
+        <v>35160000</v>
       </c>
       <c r="D12" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>231</v>
       </c>
       <c r="I12" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>35160000</v>
+        <v>35170000</v>
       </c>
       <c r="D13" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="E13" t="s">
         <v>192</v>
@@ -4186,135 +4168,135 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="I13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>35170000</v>
+        <v>35190000</v>
       </c>
       <c r="D14" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="E14" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>192</v>
+        <v>24</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="I14" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>35350000</v>
+        <v>35360000</v>
       </c>
       <c r="D15" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="E15" t="s">
         <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>258</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="I15" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>35190000</v>
+        <v>35370000</v>
       </c>
       <c r="D16" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E16" t="s">
         <v>54</v>
       </c>
-      <c r="F16" t="s">
-        <v>24</v>
+      <c r="F16">
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="I16" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>35200000</v>
+        <v>35380000</v>
       </c>
       <c r="D17" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E17" t="s">
         <v>54</v>
@@ -4326,16 +4308,16 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="I17" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -4346,206 +4328,130 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>35360000</v>
+        <v>35230000</v>
       </c>
       <c r="D18" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
       <c r="F18" t="s">
-        <v>266</v>
+        <v>40</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>249</v>
+        <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>35370000</v>
+        <v>35390000</v>
       </c>
       <c r="D19" t="s">
         <v>254</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
+        <v>192</v>
+      </c>
+      <c r="F19" t="s">
+        <v>259</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
       </c>
       <c r="H19" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="I19" t="s">
-        <v>252</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
+        <v>256</v>
+      </c>
+      <c r="J19" t="s">
+        <v>270</v>
       </c>
       <c r="K19" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>35380000</v>
+        <v>35410000</v>
       </c>
       <c r="D20" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="E20" t="s">
         <v>54</v>
       </c>
-      <c r="F20" t="s">
-        <v>24</v>
+      <c r="F20">
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="I20" t="s">
-        <v>258</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
+        <v>264</v>
+      </c>
+      <c r="J20" t="s">
+        <v>24</v>
       </c>
       <c r="K20" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>35230000</v>
+        <v>35420000</v>
       </c>
       <c r="D21" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="E21" t="s">
         <v>192</v>
       </c>
-      <c r="F21" t="s">
-        <v>40</v>
+      <c r="F21">
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
-      <c r="H21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" t="s">
-        <v>261</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
+      <c r="J21" t="s">
+        <v>24</v>
       </c>
       <c r="K21" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>265</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>35390000</v>
-      </c>
-      <c r="D22" t="s">
-        <v>262</v>
-      </c>
-      <c r="E22" t="s">
-        <v>192</v>
-      </c>
-      <c r="F22" t="s">
-        <v>267</v>
-      </c>
-      <c r="G22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" t="s">
-        <v>263</v>
-      </c>
-      <c r="I22" t="s">
-        <v>264</v>
-      </c>
-      <c r="J22" t="s">
-        <v>278</v>
-      </c>
-      <c r="K22" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>270</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>35410000</v>
-      </c>
-      <c r="D23" t="s">
-        <v>273</v>
-      </c>
-      <c r="E23" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
-        <v>271</v>
-      </c>
-      <c r="I23" t="s">
-        <v>272</v>
-      </c>
-      <c r="J23" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -4555,10 +4461,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4920,7 +4826,7 @@
         <v>186</v>
       </c>
       <c r="B45" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -4928,12 +4834,12 @@
         <v>189</v>
       </c>
       <c r="B46" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B47" t="s">
         <v>95</v>
@@ -4944,68 +4850,68 @@
         <v>195</v>
       </c>
       <c r="B48" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B49" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B50" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B51" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B52" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B53" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B54" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B55" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B56" t="s">
         <v>94</v>
@@ -5013,7 +4919,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B57" t="s">
         <v>94</v>
@@ -5021,7 +4927,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B58" t="s">
         <v>94</v>
@@ -5029,7 +4935,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B59" t="s">
         <v>94</v>
@@ -5040,39 +4946,39 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B61" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B62" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B63" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B64" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -5080,7 +4986,15 @@
         <v>102</v>
       </c>
       <c r="B65" t="s">
-        <v>276</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>279</v>
+      </c>
+      <c r="B66" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Saving updates so far for FTT-Fr
Branch does not work - just committing  freight masterfile progress.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{752E57D9-DD86-4374-B143-621D1A74ADF5}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBF05621-13DC-42AA-8AD6-D900DB38004D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -3711,7 +3711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -4463,8 +4463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4834,7 +4834,7 @@
         <v>189</v>
       </c>
       <c r="B46" t="s">
-        <v>260</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Rewrite demand from vkm
Rewrite demand, now starting from RFLZ

Rewrite the zwsa criteria to fit within new shares formulation.

Vectorise various bits and pieces, make code more DRY.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFECBA29-71FB-46E2-82AE-5307A56A82EC}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99DEB3FD-5686-411E-B667-D81B4189779D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="275">
   <si>
     <t>Variable name</t>
   </si>
@@ -614,18 +614,12 @@
     <t>RFLZ</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>Utot</t>
   </si>
   <si>
     <t>FTTI</t>
   </si>
   <si>
-    <t>FTT-Fr Demand in Million Tkm</t>
-  </si>
-  <si>
     <t>FTT-Fr Number in Fleet</t>
   </si>
   <si>
@@ -761,18 +755,6 @@
     <t>ZSFD</t>
   </si>
   <si>
-    <t>ZLOD</t>
-  </si>
-  <si>
-    <t>Costs (t/v)</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>FTT-Fr Load factors</t>
-  </si>
-  <si>
     <t>Slratio</t>
   </si>
   <si>
@@ -813,9 +795,6 @@
   </si>
   <si>
     <t xml:space="preserve">Costs </t>
-  </si>
-  <si>
-    <t>LODZ</t>
   </si>
   <si>
     <t>C6TI</t>
@@ -1256,10 +1235,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="I1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1288,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1317,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1346,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1375,7 +1354,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1404,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1433,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1462,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1476,7 +1455,7 @@
         <v>31090000</v>
       </c>
       <c r="D9" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E9" t="s">
         <v>56</v>
@@ -1491,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1520,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1549,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1578,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1607,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1636,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1665,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1694,7 +1673,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1723,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1752,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1781,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -1833,10 +1812,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="I1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1862,10 +1841,10 @@
         <v>54</v>
       </c>
       <c r="H2" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="I2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1894,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1923,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1952,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1981,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2010,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2039,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2068,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2097,7 +2076,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2126,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2155,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2184,7 +2163,7 @@
         <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2213,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2242,7 +2221,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2271,7 +2250,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2300,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2329,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2358,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2387,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2416,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2445,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2490,10 +2469,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="I1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2522,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2551,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2580,7 +2559,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2609,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2638,7 +2617,7 @@
         <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2667,7 +2646,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2696,7 +2675,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2725,7 +2704,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2754,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2783,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2812,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2841,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2870,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2899,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2928,7 +2907,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2954,10 +2933,10 @@
         <v>54</v>
       </c>
       <c r="H17" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="I17" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3003,10 +2982,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="I1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3035,7 +3014,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3064,7 +3043,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3093,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3122,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3151,7 +3130,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3180,7 +3159,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3209,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3238,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3267,7 +3246,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3296,7 +3275,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3325,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3354,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3383,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3412,7 +3391,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3441,7 +3420,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3470,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3499,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3528,7 +3507,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3557,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3586,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3615,7 +3594,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3644,7 +3623,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3673,7 +3652,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3702,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3712,10 +3691,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3757,62 +3736,62 @@
         <v>188</v>
       </c>
       <c r="J1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="K1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>35330000</v>
+        <v>35320000</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>273</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="s">
+        <v>54</v>
       </c>
       <c r="H2" t="s">
         <v>190</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>35320000</v>
+        <v>35060000</v>
       </c>
       <c r="D3" t="s">
         <v>194</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>191</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -3821,77 +3800,77 @@
         <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>270</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>35060000</v>
+        <v>35140000</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="E4" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
-        <v>54</v>
+      <c r="G4">
+        <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>195</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>277</v>
+        <v>213</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>35140000</v>
+        <v>35040000</v>
       </c>
       <c r="D5" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="G5">
-        <v>0</v>
+      <c r="G5" t="s">
+        <v>54</v>
       </c>
       <c r="H5" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="I5" t="s">
         <v>197</v>
@@ -3900,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3911,13 +3890,13 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>35040000</v>
+        <v>35050000</v>
       </c>
       <c r="D6" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="E6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -3926,68 +3905,68 @@
         <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="I6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>35050000</v>
+        <v>35020000</v>
       </c>
       <c r="D7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>211</v>
+      </c>
+      <c r="I7" t="s">
         <v>203</v>
       </c>
-      <c r="E7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" t="s">
-        <v>201</v>
-      </c>
-      <c r="I7" t="s">
-        <v>204</v>
-      </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>35020000</v>
+        <v>35030000</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="E8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -3996,65 +3975,65 @@
         <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="I8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>35030000</v>
+        <v>35150000</v>
       </c>
       <c r="D9" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E9" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" t="s">
-        <v>54</v>
+      <c r="G9">
+        <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="I9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>35150000</v>
+        <v>35130000</v>
       </c>
       <c r="D10" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
@@ -4066,167 +4045,167 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>210</v>
+        <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>35130000</v>
+        <v>35160000</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>191</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>229</v>
       </c>
       <c r="I11" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>35160000</v>
+        <v>35170000</v>
       </c>
       <c r="D12" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="E12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="I12" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>35170000</v>
+        <v>35190000</v>
       </c>
       <c r="D13" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="E13" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>192</v>
+        <v>24</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="I13" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>35190000</v>
+        <v>35370000</v>
       </c>
       <c r="D14" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="E14" t="s">
         <v>54</v>
       </c>
-      <c r="F14" t="s">
-        <v>24</v>
+      <c r="F14">
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I14" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>35360000</v>
+        <v>35380000</v>
       </c>
       <c r="D15" t="s">
         <v>242</v>
@@ -4235,80 +4214,80 @@
         <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>257</v>
+        <v>24</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="I15" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>35370000</v>
+        <v>35230000</v>
       </c>
       <c r="D16" t="s">
         <v>246</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
+        <v>191</v>
+      </c>
+      <c r="F16" t="s">
+        <v>40</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>243</v>
+        <v>35</v>
       </c>
       <c r="I16" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>35380000</v>
+        <v>35390000</v>
       </c>
       <c r="D17" t="s">
         <v>248</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
+        <v>251</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
       </c>
       <c r="H17" t="s">
         <v>249</v>
@@ -4316,145 +4295,75 @@
       <c r="I17" t="s">
         <v>250</v>
       </c>
-      <c r="J17">
-        <v>0</v>
+      <c r="J17" t="s">
+        <v>262</v>
       </c>
       <c r="K17" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>35230000</v>
+        <v>35410000</v>
       </c>
       <c r="D18" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E18" t="s">
-        <v>192</v>
-      </c>
-      <c r="F18" t="s">
-        <v>40</v>
+        <v>54</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>35</v>
+        <v>255</v>
       </c>
       <c r="I18" t="s">
-        <v>253</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
+        <v>256</v>
+      </c>
+      <c r="J18" t="s">
+        <v>24</v>
       </c>
       <c r="K18" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>35390000</v>
+        <v>35420000</v>
       </c>
       <c r="D19" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
-      </c>
-      <c r="F19" t="s">
-        <v>258</v>
-      </c>
-      <c r="G19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" t="s">
-        <v>255</v>
-      </c>
-      <c r="I19" t="s">
-        <v>256</v>
+        <v>191</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>269</v>
+        <v>24</v>
       </c>
       <c r="K19" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>261</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>35410000</v>
-      </c>
-      <c r="D20" t="s">
-        <v>264</v>
-      </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>262</v>
-      </c>
-      <c r="I20" t="s">
-        <v>263</v>
-      </c>
-      <c r="J20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>278</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>35420000</v>
-      </c>
-      <c r="D21" t="s">
-        <v>279</v>
-      </c>
-      <c r="E21" t="s">
-        <v>192</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -4829,7 +4738,7 @@
         <v>186</v>
       </c>
       <c r="B45" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -4842,7 +4751,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B47" t="s">
         <v>95</v>
@@ -4850,71 +4759,71 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B48" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B49" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B50" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B51" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B52" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B53" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B54" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B55" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B56" t="s">
         <v>94</v>
@@ -4922,7 +4831,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B57" t="s">
         <v>94</v>
@@ -4930,7 +4839,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B58" t="s">
         <v>94</v>
@@ -4938,7 +4847,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B59" t="s">
         <v>94</v>
@@ -4949,39 +4858,39 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B61" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B62" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B63" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B64" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -4989,15 +4898,15 @@
         <v>102</v>
       </c>
       <c r="B65" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B66" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>